<commit_message>
All Test methods Implemented Feb 14th CheckIn
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AspireQACodeChallenge1202\AspireQACodeChallenge\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18297A48-3FFE-4BA8-B948-D4D3FB640310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B480EA-B57D-4D99-B828-738AC6CCEC88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Fileds</t>
   </si>
@@ -55,20 +57,58 @@
     <t>thiru</t>
   </si>
   <si>
-    <t>Q1234</t>
-  </si>
-  <si>
     <t>FirstRecord</t>
+  </si>
+  <si>
+    <t>Mobile Num</t>
+  </si>
+  <si>
+    <t>OTP</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>thirumala123@gmail.com</t>
+  </si>
+  <si>
+    <t>Invalid</t>
+  </si>
+  <si>
+    <t>Valid</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>+919090909090</t>
+  </si>
+  <si>
+    <t>+6520222022</t>
+  </si>
+  <si>
+    <t>+914040404040</t>
+  </si>
+  <si>
+    <t>thirumala.kiran85@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -106,15 +146,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -395,14 +438,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" customWidth="1"/>
     <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -421,7 +466,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
@@ -430,10 +475,112 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2347B062-CDB7-4BE1-884F-035618365B14}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31A32EDD-9983-41DB-8F9B-0427154A8C9F}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{448532B9-0130-4614-8B86-970D31A387ED}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{6AA02040-FB87-4936-A0DD-4924623E2DCE}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>